<commit_message>
Relations between tables (entity)
</commit_message>
<xml_diff>
--- a/Projekt Dom.xlsx
+++ b/Projekt Dom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkozakowski\Desktop\KODY\HouseProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D63C77-0152-4E42-871D-31F6FE5EAD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D32DC5B-74A9-452A-97FA-D3A6CE2B5904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30195" yWindow="390" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EtapI " sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="101">
   <si>
     <t>Projekt i przygotowanie do budowy</t>
   </si>
@@ -224,15 +224,6 @@
     <t>urząd gminy</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>subtype</t>
-  </si>
-  <si>
-    <t>recipient</t>
-  </si>
-  <si>
     <t>sent via</t>
   </si>
   <si>
@@ -254,9 +245,6 @@
     <t>contact</t>
   </si>
   <si>
-    <t>payment</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -339,6 +327,12 @@
   </si>
   <si>
     <t>finish</t>
+  </si>
+  <si>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>sent type</t>
   </si>
 </sst>
 </file>
@@ -475,12 +469,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -490,10 +479,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
@@ -2166,7 +2160,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2174,22 +2168,22 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2239,28 +2233,28 @@
         <v>15</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="F15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2292,245 +2286,218 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75C9D0E-4145-4493-89D4-3795922CA11D}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" customWidth="1"/>
-    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G2" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="K3" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="J3" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="6" t="s">
+      <c r="M4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>74</v>
-      </c>
       <c r="P4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C12" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>75</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="K13" s="10" t="s">
-        <v>75</v>
-      </c>
+      <c r="J13" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>9</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E14" t="s">
         <v>57</v>
       </c>
-      <c r="K14" t="s">
+      <c r="J14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>1</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" t="s">
         <v>58</v>
       </c>
-      <c r="K15" t="s">
+      <c r="J15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F16" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
         <v>59</v>
       </c>
-      <c r="K16" t="s">
+      <c r="J16" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="J3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2541,7 +2508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A727703-7957-401C-9729-874D76FB55E3}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2562,23 +2529,23 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E2" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="E2" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="13"/>
+      <c r="A3" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="17"/>
       <c r="E3" s="3" t="s">
         <v>25</v>
       </c>
@@ -2612,7 +2579,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>24</v>
@@ -2633,7 +2600,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>26</v>
@@ -2654,7 +2621,7 @@
         <v>38</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>27</v>
@@ -2675,7 +2642,7 @@
         <v>42</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>39</v>
@@ -2784,7 +2751,7 @@
   <dimension ref="B1:N9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2798,45 +2765,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="L1" s="12"/>
-      <c r="M1" s="13"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="B2" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>43</v>
@@ -2904,7 +2871,7 @@
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
@@ -2926,8 +2893,8 @@
       <c r="G2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="13"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="7"/>
@@ -2937,7 +2904,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="K3" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="L3" s="11"/>
     </row>

</xml_diff>

<commit_message>
Dependency injection services per project
</commit_message>
<xml_diff>
--- a/Projekt Dom.xlsx
+++ b/Projekt Dom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkozakowski\Desktop\KODY\HouseProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D32DC5B-74A9-452A-97FA-D3A6CE2B5904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB847F05-C889-4695-9F62-81431ED85E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30195" yWindow="390" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="100">
   <si>
     <t>Projekt i przygotowanie do budowy</t>
   </si>
@@ -252,9 +252,6 @@
   </si>
   <si>
     <t>payment type</t>
-  </si>
-  <si>
-    <t>total cost</t>
   </si>
   <si>
     <t>advance</t>
@@ -2124,7 +2121,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,7 +2157,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2183,7 +2180,7 @@
         <v>68</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2233,7 +2230,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2245,16 +2242,16 @@
         <v>72</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>73</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2317,7 +2314,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -2326,7 +2323,7 @@
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="J3" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
@@ -2343,7 +2340,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>66</v>
@@ -2352,7 +2349,7 @@
         <v>68</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>2</v>
@@ -2379,7 +2376,7 @@
         <v>69</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -2432,7 +2429,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C12" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12" t="s">
@@ -2442,7 +2439,7 @@
       <c r="H12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
@@ -2530,7 +2527,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E2" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -2543,7 +2540,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="17"/>
       <c r="E3" s="3" t="s">
@@ -2579,7 +2576,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>24</v>
@@ -2600,7 +2597,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>26</v>
@@ -2621,7 +2618,7 @@
         <v>38</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>27</v>
@@ -2642,7 +2639,7 @@
         <v>42</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>39</v>
@@ -2770,7 +2767,7 @@
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -2788,22 +2785,22 @@
         <v>71</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>73</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>43</v>
@@ -2871,7 +2868,7 @@
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
@@ -2904,7 +2901,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="K3" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L3" s="11"/>
     </row>

</xml_diff>

<commit_message>
added material and execution table
</commit_message>
<xml_diff>
--- a/Projekt Dom.xlsx
+++ b/Projekt Dom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkozakowski\Desktop\KODY\HouseProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB847F05-C889-4695-9F62-81431ED85E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD3A5A9-B22B-45CE-9E4C-34F12E003A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30195" yWindow="390" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EtapI " sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="101">
   <si>
     <t>Projekt i przygotowanie do budowy</t>
   </si>
@@ -92,9 +92,6 @@
     <t xml:space="preserve">1. </t>
   </si>
   <si>
-    <t>zaliczka</t>
-  </si>
-  <si>
     <t>otwarty</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>ściany nośne</t>
   </si>
   <si>
-    <t>ZADANIE</t>
-  </si>
-  <si>
     <t>strop</t>
   </si>
   <si>
@@ -131,15 +125,6 @@
     <t>okna</t>
   </si>
   <si>
-    <t>materiały</t>
-  </si>
-  <si>
-    <t>koszt szacowany</t>
-  </si>
-  <si>
-    <t>koszt poniesiony</t>
-  </si>
-  <si>
     <t>data rozpoczęcia</t>
   </si>
   <si>
@@ -330,6 +315,24 @@
   </si>
   <si>
     <t>sent type</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>work stage</t>
+  </si>
+  <si>
+    <t>materials</t>
+  </si>
+  <si>
+    <t>estimated cost</t>
+  </si>
+  <si>
+    <t>cost payed</t>
+  </si>
+  <si>
+    <t>account</t>
   </si>
 </sst>
 </file>
@@ -2157,7 +2160,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2165,22 +2168,22 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2189,7 +2192,7 @@
         <v>12</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>3</v>
@@ -2230,28 +2233,28 @@
         <v>15</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="F15" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2285,7 +2288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75C9D0E-4145-4493-89D4-3795922CA11D}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -2314,7 +2317,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -2323,7 +2326,7 @@
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="J3" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
@@ -2337,46 +2340,46 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="P4" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -2429,33 +2432,33 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C12" s="12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="J13" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
@@ -2466,10 +2469,10 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -2477,18 +2480,18 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="J15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2505,8 +2508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A727703-7957-401C-9729-874D76FB55E3}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2514,6 +2517,8 @@
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -2522,12 +2527,12 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E2" s="15" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -2540,35 +2545,35 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B3" s="17"/>
       <c r="E3" s="3" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="L3" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2576,13 +2581,13 @@
         <v>19</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
@@ -2594,16 +2599,16 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -2615,16 +2620,16 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
@@ -2636,16 +2641,16 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -2657,10 +2662,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E8" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -2672,10 +2677,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E9" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -2687,10 +2692,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E10" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
@@ -2702,10 +2707,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E11" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -2717,10 +2722,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E12" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -2745,29 +2750,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1F9902-63EE-4298-B4C5-D00DCD387858}">
-  <dimension ref="B1:N9"/>
+  <dimension ref="B1:O9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="L1" s="16"/>
-      <c r="M1" s="17"/>
-    </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M1" s="16"/>
+      <c r="N1" s="17"/>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -2776,73 +2781,79 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
-      <c r="L2" s="4"/>
+      <c r="J2" s="18"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J3" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
-        <v>46</v>
-      </c>
+      <c r="G5" s="10"/>
       <c r="H5" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J9" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2868,27 +2879,27 @@
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="K2" s="16"/>
       <c r="L2" s="17"/>
@@ -2901,7 +2912,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="K3" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="L3" s="11"/>
     </row>
@@ -2910,24 +2921,24 @@
         <v>11</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="K5" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="L5" s="7"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="K6" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="L6" s="7"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="K7" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="L7" s="7"/>
     </row>

</xml_diff>

<commit_message>
added Finance table to entity
</commit_message>
<xml_diff>
--- a/Projekt Dom.xlsx
+++ b/Projekt Dom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkozakowski\Desktop\KODY\HouseProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD3A5A9-B22B-45CE-9E4C-34F12E003A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB72C193-E605-487B-93F9-D2835BCB394C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EtapI " sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="102">
   <si>
     <t>Projekt i przygotowanie do budowy</t>
   </si>
@@ -125,21 +125,12 @@
     <t>okna</t>
   </si>
   <si>
-    <t>data rozpoczęcia</t>
-  </si>
-  <si>
-    <t>data zakończenia</t>
-  </si>
-  <si>
     <t>3.</t>
   </si>
   <si>
     <t>pokrycie dachu</t>
   </si>
   <si>
-    <t>koszt robocizny</t>
-  </si>
-  <si>
     <t>Etap: stan</t>
   </si>
   <si>
@@ -333,6 +324,18 @@
   </si>
   <si>
     <t>account</t>
+  </si>
+  <si>
+    <t>labor cost (koszt robocizny)</t>
+  </si>
+  <si>
+    <t>StartedAt</t>
+  </si>
+  <si>
+    <t>FinishedAt</t>
+  </si>
+  <si>
+    <t>Savings</t>
   </si>
 </sst>
 </file>
@@ -2160,7 +2163,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2168,22 +2171,22 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2192,7 +2195,7 @@
         <v>12</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>3</v>
@@ -2233,28 +2236,28 @@
         <v>15</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="F15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2317,7 +2320,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -2326,7 +2329,7 @@
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="J3" s="14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
@@ -2340,46 +2343,46 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="P4" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -2432,33 +2435,33 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C12" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="J13" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
@@ -2469,10 +2472,10 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -2480,18 +2483,18 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2508,8 +2511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A727703-7957-401C-9729-874D76FB55E3}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,18 +2524,19 @@
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E2" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -2545,35 +2549,35 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="17"/>
       <c r="E3" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2581,7 +2585,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>23</v>
@@ -2602,7 +2606,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>24</v>
@@ -2620,10 +2624,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>25</v>
@@ -2641,13 +2645,13 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>20</v>
@@ -2772,7 +2776,7 @@
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -2788,31 +2792,31 @@
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="J3" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
@@ -2826,7 +2830,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J4" s="10"/>
     </row>
@@ -2838,16 +2842,16 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J5" s="10"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2863,7 +2867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1A8AD6F-014B-4E38-BEDF-0A36BBC252A6}">
   <dimension ref="B1:L7"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2879,27 +2883,27 @@
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K2" s="16"/>
       <c r="L2" s="17"/>
@@ -2912,7 +2916,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="K3" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L3" s="11"/>
     </row>
@@ -2921,24 +2925,24 @@
         <v>11</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="K5" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L5" s="7"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="K6" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L6" s="7"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="K7" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L7" s="7"/>
     </row>

</xml_diff>

<commit_message>
Update execution, notification event after adding material
</commit_message>
<xml_diff>
--- a/Projekt Dom.xlsx
+++ b/Projekt Dom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\source\repos\HouseProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2A4826-3E6C-4CA6-97E5-175F83656E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFFD498-47AD-4266-B45C-4F5E95988CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="111">
   <si>
     <t>Projekt i przygotowanie do budowy</t>
   </si>
@@ -318,9 +318,6 @@
     <t>cost payed</t>
   </si>
   <si>
-    <t>account</t>
-  </si>
-  <si>
     <t>labor cost (koszt robocizny)</t>
   </si>
   <si>
@@ -367,6 +364,12 @@
   </si>
   <si>
     <t>brama, ogrodzenie</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>=koszt materiałów(amount * price unit) + A</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -534,6 +537,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
@@ -2552,10 +2556,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A727703-7957-401C-9729-874D76FB55E3}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2568,16 +2572,16 @@
     <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E2" s="17" t="s">
         <v>72</v>
       </c>
@@ -2588,9 +2592,8 @@
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>71</v>
       </c>
@@ -2608,22 +2611,19 @@
         <v>91</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>92</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>19</v>
       </c>
@@ -2638,13 +2638,16 @@
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="I4" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>110</v>
+      </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
@@ -2663,9 +2666,8 @@
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
@@ -2684,9 +2686,8 @@
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>34</v>
       </c>
@@ -2705,9 +2706,8 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E8" s="9" t="s">
         <v>26</v>
       </c>
@@ -2720,9 +2720,8 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E9" s="9" t="s">
         <v>27</v>
       </c>
@@ -2735,9 +2734,8 @@
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E10" s="9" t="s">
         <v>28</v>
       </c>
@@ -2750,9 +2748,8 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
@@ -2762,12 +2759,10 @@
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E12" s="9" t="s">
         <v>30</v>
       </c>
@@ -2777,38 +2772,36 @@
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E13" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F13" s="9" t="s">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E14" s="9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E14" s="9" t="s">
+      <c r="F14" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E15" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E15" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E16" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>85</v>
@@ -2816,12 +2809,12 @@
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E2:M2"/>
+    <mergeCell ref="E2:L2"/>
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2969,28 +2962,28 @@
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>39</v>
       </c>
       <c r="F2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>103</v>
-      </c>
       <c r="I2" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Upadate Finance: by document and by execution
</commit_message>
<xml_diff>
--- a/Projekt Dom.xlsx
+++ b/Projekt Dom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkozakowski\Desktop\KODY\HouseProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D04D67C-F4C6-44BE-A56B-4835620C8A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99496D73-98F6-4CCD-B3C7-1F2FD0B4B547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EtapI " sheetId="1" r:id="rId1"/>
@@ -478,6 +478,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -496,8 +498,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
@@ -2133,8 +2133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2299,7 +2299,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2326,24 +2326,24 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="J3" s="14" t="s">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="J3" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2518,8 +2518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A727703-7957-401C-9729-874D76FB55E3}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2542,22 +2542,22 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="17"/>
+      <c r="B3" s="19"/>
       <c r="E3" s="3" t="s">
         <v>58</v>
       </c>
@@ -2801,20 +2801,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="N1" s="19"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
       <c r="M2" s="10" t="s">
         <v>78</v>
       </c>
@@ -2946,38 +2946,38 @@
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Delete Application table and move attachments to documents
</commit_message>
<xml_diff>
--- a/Projekt Dom.xlsx
+++ b/Projekt Dom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkozakowski\Desktop\KODY\HouseProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99496D73-98F6-4CCD-B3C7-1F2FD0B4B547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D917DD-B056-4E22-B7D9-24242ED49AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="2310" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EtapI " sheetId="1" r:id="rId1"/>
@@ -2133,7 +2133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -2296,10 +2296,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75C9D0E-4145-4493-89D4-3795922CA11D}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2444,18 +2444,9 @@
       <c r="C12" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11" t="s">
+      <c r="E12" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
@@ -2464,15 +2455,6 @@
       <c r="E13" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="J13" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
@@ -2481,9 +2463,6 @@
       <c r="E14" t="s">
         <v>44</v>
       </c>
-      <c r="J14" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
@@ -2492,15 +2471,34 @@
       <c r="E15" t="s">
         <v>45</v>
       </c>
-      <c r="J15" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>46</v>
       </c>
-      <c r="J16" t="s">
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2519,7 +2517,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Getting attachments in document
</commit_message>
<xml_diff>
--- a/Projekt Dom.xlsx
+++ b/Projekt Dom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkozakowski\Desktop\KODY\HouseProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D917DD-B056-4E22-B7D9-24242ED49AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDDE5A6-DD5D-440D-9A99-8CB5C96F9C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="2310" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EtapI " sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="99">
   <si>
     <t>Projekt i przygotowanie do budowy</t>
   </si>
@@ -60,9 +60,6 @@
     <t>…</t>
   </si>
   <si>
-    <t>e-mail/ poczta…</t>
-  </si>
-  <si>
     <t xml:space="preserve">2. </t>
   </si>
   <si>
@@ -192,27 +189,18 @@
     <t>urząd gminy</t>
   </si>
   <si>
-    <t>sent via</t>
-  </si>
-  <si>
     <t>SEND_TYPE</t>
   </si>
   <si>
     <t>post</t>
   </si>
   <si>
-    <t>send at</t>
-  </si>
-  <si>
     <t>received at</t>
   </si>
   <si>
     <t>cost</t>
   </si>
   <si>
-    <t>contact</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -229,9 +217,6 @@
   </si>
   <si>
     <t>DOCUMENTS</t>
-  </si>
-  <si>
-    <t>APPLICATIONS</t>
   </si>
   <si>
     <t>POSTS</t>
@@ -383,7 +368,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,18 +384,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -472,17 +445,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -495,7 +464,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2167,57 +2136,57 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2240,49 +2209,49 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2296,10 +2265,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75C9D0E-4145-4493-89D4-3795922CA11D}">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2309,114 +2278,80 @@
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="J3" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="B4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2424,7 +2359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2432,7 +2367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2440,72 +2375,71 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C13" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>1</v>
       </c>
       <c r="E15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>46</v>
-      </c>
-    </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="11" t="s">
-        <v>65</v>
+      <c r="C20" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="9" t="s">
-        <v>58</v>
+      <c r="C21" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="J3:P3"/>
+  <mergeCells count="1">
+    <mergeCell ref="B3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2536,238 +2470,238 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="E3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E2" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="19"/>
-      <c r="E3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="B7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E13" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="F13" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E14" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="F14" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="K3" s="3" t="s">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E15" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="F15" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E16" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E13" s="9" t="s">
+      <c r="F16" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E14" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E15" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E16" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="9" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2799,113 +2733,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="N1" s="13"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="M2" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="N2" s="10"/>
+      <c r="B2" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="M2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="J3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N3" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="M4" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="9"/>
-      <c r="M4" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="N4" s="7"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
+      <c r="J5" s="8"/>
+      <c r="M5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="9"/>
-      <c r="M5" s="7" t="s">
+      <c r="N5" s="6"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="7"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M6" s="7" t="s">
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="7"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="N7" s="7"/>
+      <c r="N7" s="6"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2939,43 +2873,43 @@
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E1" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Unit tests  - Documents
</commit_message>
<xml_diff>
--- a/Projekt Dom.xlsx
+++ b/Projekt Dom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkozakowski\Desktop\KODY\HouseProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDDE5A6-DD5D-440D-9A99-8CB5C96F9C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA461BC3-F65A-4ABC-BBEE-F6D50D450F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EtapI " sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="98">
   <si>
     <t>Projekt i przygotowanie do budowy</t>
   </si>
@@ -327,13 +327,10 @@
     <t>brama, ogrodzenie</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>=koszt materiałów(amount * price unit) + A</t>
-  </si>
-  <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>=material_cost(amount * price unit) + labor cost</t>
   </si>
 </sst>
 </file>
@@ -2102,7 +2099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -2267,7 +2264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75C9D0E-4145-4493-89D4-3795922CA11D}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -2451,7 +2448,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2459,7 +2456,7 @@
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
@@ -2530,9 +2527,7 @@
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="8" t="s">
-        <v>96</v>
-      </c>
+      <c r="I4" s="8"/>
       <c r="J4" s="11" t="s">
         <v>97</v>
       </c>
@@ -2651,6 +2646,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
     </row>
@@ -2664,6 +2660,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
     </row>
@@ -2674,6 +2671,12 @@
       <c r="F13" s="8" t="s">
         <v>91</v>
       </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E14" s="8" t="s">
@@ -2682,6 +2685,12 @@
       <c r="F14" s="8" t="s">
         <v>91</v>
       </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E15" s="8" t="s">
@@ -2690,6 +2699,12 @@
       <c r="F15" s="8" t="s">
         <v>79</v>
       </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E16" s="8" t="s">
@@ -2698,11 +2713,26 @@
       <c r="F16" s="8" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" s="8" t="s">
         <v>95</v>
       </c>
+      <c r="F17" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2802,7 +2832,7 @@
       </c>
       <c r="J4" s="8"/>
       <c r="M4" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="N4" s="6"/>
     </row>

</xml_diff>